<commit_message>
can do json transmission between esp to server and server to client, ongoing with map, yet to do status display and layout
</commit_message>
<xml_diff>
--- a/Project_Management_Mars Rover 2022.xlsx
+++ b/Project_Management_Mars Rover 2022.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ab10216_ic_ac_uk/Documents/1-Imperial College London/2-Teaching Fellow/2-TF 21-22/2nd year/1-Mars Rover 2022/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christinawang/Desktop/MarsRover_git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{2A809C9D-E205-4366-AF60-0802B965C325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABBC2AF4-E732-47EF-BD54-AE66B8F8BD8D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E97D915-86AC-AD4A-AC6C-EBF8E215332B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="11" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Gantt Chart'!$1:$12</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Gantt Chart'!$4:$6</definedName>
     <definedName name="task_end" localSheetId="0">'Gantt Chart'!$F1</definedName>
     <definedName name="task_progress" localSheetId="0">'Gantt Chart'!$D1</definedName>
     <definedName name="task_start" localSheetId="0">'Gantt Chart'!$E1</definedName>
     <definedName name="today" localSheetId="0">'Gantt Chart'!$E$3</definedName>
     <definedName name="valuevx">42.314159</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Gantt Chart'!$1:$12</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -83,9 +83,6 @@
     <t>Mars Rover 2022</t>
   </si>
   <si>
-    <t>Group X</t>
-  </si>
-  <si>
     <t>Project Start:</t>
   </si>
   <si>
@@ -130,6 +127,9 @@
   <si>
     <t>Title 2</t>
   </si>
+  <si>
+    <t>Group 8</t>
+  </si>
 </sst>
 </file>
 
@@ -141,11 +141,11 @@
     <numFmt numFmtId="166" formatCode="d"/>
     <numFmt numFmtId="167" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -153,13 +153,13 @@
       <b/>
       <sz val="20"/>
       <color theme="4" tint="-0.249977111117893"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -172,7 +172,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -180,7 +180,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -188,34 +188,34 @@
       <b/>
       <sz val="9"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="0" tint="-0.499984740745262"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -235,7 +235,7 @@
     <font>
       <sz val="8"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -243,14 +243,14 @@
       <b/>
       <sz val="22"/>
       <color theme="1" tint="0.34998626667073579"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -600,29 +600,29 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Pourcentage" xfId="2" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="15">
     <dxf>
@@ -1152,24 +1152,24 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="68" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.75" customWidth="1"/>
-    <col min="2" max="2" width="69.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.25" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="64" width="2.625" customWidth="1"/>
-    <col min="69" max="70" width="10.25"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="69.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="64" width="2.6640625" customWidth="1"/>
+    <col min="69" max="70" width="10.1640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="28.15">
+    <row r="1" spans="1:64" ht="29" x14ac:dyDescent="0.35">
       <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1179,139 +1179,139 @@
       <c r="F1" s="34"/>
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="49"/>
-      <c r="S1" s="49"/>
-      <c r="T1" s="49"/>
-      <c r="U1" s="49"/>
-      <c r="V1" s="49"/>
-      <c r="W1" s="49"/>
-      <c r="X1" s="49"/>
-      <c r="Y1" s="49"/>
-      <c r="Z1" s="49"/>
-      <c r="AA1" s="49"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="54"/>
     </row>
-    <row r="2" spans="1:64" ht="19.5" customHeight="1">
+    <row r="2" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="49">
+        <v>44704</v>
+      </c>
+      <c r="F2" s="50"/>
+    </row>
+    <row r="3" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="53">
-        <v>44704</v>
-      </c>
-      <c r="F2" s="54"/>
+      <c r="D3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="49">
+        <f ca="1">TODAY()</f>
+        <v>44707</v>
+      </c>
+      <c r="F3" s="50"/>
     </row>
-    <row r="3" spans="1:64" ht="19.5" customHeight="1">
-      <c r="B3" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="6" t="s">
+    <row r="4" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D4" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="E3" s="53">
-        <f ca="1">TODAY()</f>
-        <v>44704</v>
-      </c>
-      <c r="F3" s="54"/>
-    </row>
-    <row r="4" spans="1:64" ht="19.5" customHeight="1">
-      <c r="D4" s="6" t="s">
-        <v>5</v>
       </c>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="50">
+      <c r="I4" s="51">
         <f>I5</f>
         <v>44704</v>
       </c>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="52"/>
-      <c r="P4" s="50">
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="52"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="52"/>
+      <c r="O4" s="53"/>
+      <c r="P4" s="51">
         <f>P5</f>
         <v>44711</v>
       </c>
-      <c r="Q4" s="51"/>
-      <c r="R4" s="51"/>
-      <c r="S4" s="51"/>
-      <c r="T4" s="51"/>
-      <c r="U4" s="51"/>
-      <c r="V4" s="52"/>
-      <c r="W4" s="50">
+      <c r="Q4" s="52"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="52"/>
+      <c r="T4" s="52"/>
+      <c r="U4" s="52"/>
+      <c r="V4" s="53"/>
+      <c r="W4" s="51">
         <f>W5</f>
         <v>44718</v>
       </c>
-      <c r="X4" s="51"/>
-      <c r="Y4" s="51"/>
-      <c r="Z4" s="51"/>
-      <c r="AA4" s="51"/>
-      <c r="AB4" s="51"/>
-      <c r="AC4" s="52"/>
-      <c r="AD4" s="50">
+      <c r="X4" s="52"/>
+      <c r="Y4" s="52"/>
+      <c r="Z4" s="52"/>
+      <c r="AA4" s="52"/>
+      <c r="AB4" s="52"/>
+      <c r="AC4" s="53"/>
+      <c r="AD4" s="51">
         <f>AD5</f>
         <v>44725</v>
       </c>
-      <c r="AE4" s="51"/>
-      <c r="AF4" s="51"/>
-      <c r="AG4" s="51"/>
-      <c r="AH4" s="51"/>
-      <c r="AI4" s="51"/>
-      <c r="AJ4" s="52"/>
-      <c r="AK4" s="50">
+      <c r="AE4" s="52"/>
+      <c r="AF4" s="52"/>
+      <c r="AG4" s="52"/>
+      <c r="AH4" s="52"/>
+      <c r="AI4" s="52"/>
+      <c r="AJ4" s="53"/>
+      <c r="AK4" s="51">
         <f>AK5</f>
         <v>44732</v>
       </c>
-      <c r="AL4" s="51"/>
-      <c r="AM4" s="51"/>
-      <c r="AN4" s="51"/>
-      <c r="AO4" s="51"/>
-      <c r="AP4" s="51"/>
-      <c r="AQ4" s="52"/>
-      <c r="AR4" s="50">
+      <c r="AL4" s="52"/>
+      <c r="AM4" s="52"/>
+      <c r="AN4" s="52"/>
+      <c r="AO4" s="52"/>
+      <c r="AP4" s="52"/>
+      <c r="AQ4" s="53"/>
+      <c r="AR4" s="51">
         <f>AR5</f>
         <v>44739</v>
       </c>
-      <c r="AS4" s="51"/>
-      <c r="AT4" s="51"/>
-      <c r="AU4" s="51"/>
-      <c r="AV4" s="51"/>
-      <c r="AW4" s="51"/>
-      <c r="AX4" s="52"/>
-      <c r="AY4" s="50">
+      <c r="AS4" s="52"/>
+      <c r="AT4" s="52"/>
+      <c r="AU4" s="52"/>
+      <c r="AV4" s="52"/>
+      <c r="AW4" s="52"/>
+      <c r="AX4" s="53"/>
+      <c r="AY4" s="51">
         <f>AY5</f>
         <v>44746</v>
       </c>
-      <c r="AZ4" s="51"/>
-      <c r="BA4" s="51"/>
-      <c r="BB4" s="51"/>
-      <c r="BC4" s="51"/>
-      <c r="BD4" s="51"/>
-      <c r="BE4" s="52"/>
-      <c r="BF4" s="50">
+      <c r="AZ4" s="52"/>
+      <c r="BA4" s="52"/>
+      <c r="BB4" s="52"/>
+      <c r="BC4" s="52"/>
+      <c r="BD4" s="52"/>
+      <c r="BE4" s="53"/>
+      <c r="BF4" s="51">
         <f>BF5</f>
         <v>44753</v>
       </c>
-      <c r="BG4" s="51"/>
-      <c r="BH4" s="51"/>
-      <c r="BI4" s="51"/>
-      <c r="BJ4" s="51"/>
-      <c r="BK4" s="51"/>
-      <c r="BL4" s="52"/>
+      <c r="BG4" s="52"/>
+      <c r="BH4" s="52"/>
+      <c r="BI4" s="52"/>
+      <c r="BJ4" s="52"/>
+      <c r="BK4" s="52"/>
+      <c r="BL4" s="53"/>
     </row>
-    <row r="5" spans="1:64">
+    <row r="5" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="G5" s="6"/>
       <c r="I5" s="13">
@@ -1539,26 +1539,26 @@
         <v>44759</v>
       </c>
     </row>
-    <row r="6" spans="1:64" ht="29.25" customHeight="1" thickBot="1">
+    <row r="6" spans="1:64" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="D6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="E6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="F6" s="11" t="s">
         <v>9</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>10</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I6" s="15" t="str">
         <f t="shared" ref="I6" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
@@ -1785,7 +1785,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="7" spans="1:64" s="3" customFormat="1" ht="21" thickBot="1">
+    <row r="7" spans="1:64" s="3" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17"/>
       <c r="B7" s="18"/>
       <c r="C7" s="19"/>
@@ -1794,7 +1794,7 @@
       <c r="F7" s="22"/>
       <c r="G7" s="23"/>
       <c r="H7" s="23" t="str">
-        <f t="shared" ref="H7:H12" ca="1" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H7:H12" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I7" s="32"/>
@@ -1854,10 +1854,10 @@
       <c r="BK7" s="32"/>
       <c r="BL7" s="32"/>
     </row>
-    <row r="8" spans="1:64" s="3" customFormat="1" ht="21" thickBot="1">
+    <row r="8" spans="1:64" s="3" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17"/>
       <c r="B8" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="25"/>
       <c r="D8" s="26"/>
@@ -1865,7 +1865,7 @@
       <c r="F8" s="28"/>
       <c r="G8" s="23"/>
       <c r="H8" s="23" t="str">
-        <f t="shared" ref="H8:H17" ca="1" si="7">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H17" si="7">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="32"/>
@@ -1925,10 +1925,10 @@
       <c r="BK8" s="32"/>
       <c r="BL8" s="32"/>
     </row>
-    <row r="9" spans="1:64" s="3" customFormat="1" ht="21" thickBot="1">
+    <row r="9" spans="1:64" s="3" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="30"/>
       <c r="D9" s="31">
@@ -1942,7 +1942,7 @@
       </c>
       <c r="G9" s="23"/>
       <c r="H9" s="23">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="I9" s="32"/>
@@ -2002,10 +2002,10 @@
       <c r="BK9" s="32"/>
       <c r="BL9" s="32"/>
     </row>
-    <row r="10" spans="1:64" s="3" customFormat="1" ht="21" thickBot="1">
+    <row r="10" spans="1:64" s="3" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="B10" s="29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="30"/>
       <c r="D10" s="31">
@@ -2019,7 +2019,7 @@
       </c>
       <c r="G10" s="23"/>
       <c r="H10" s="23">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" si="7"/>
         <v>14</v>
       </c>
       <c r="I10" s="32"/>
@@ -2079,10 +2079,10 @@
       <c r="BK10" s="32"/>
       <c r="BL10" s="32"/>
     </row>
-    <row r="11" spans="1:64" s="3" customFormat="1" ht="21" thickBot="1">
+    <row r="11" spans="1:64" s="3" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" s="37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="30"/>
       <c r="D11" s="31">
@@ -2096,7 +2096,7 @@
       </c>
       <c r="G11" s="23"/>
       <c r="H11" s="23">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I11" s="32"/>
@@ -2156,7 +2156,7 @@
       <c r="BK11" s="32"/>
       <c r="BL11" s="32"/>
     </row>
-    <row r="12" spans="1:64" s="3" customFormat="1" ht="21" thickBot="1">
+    <row r="12" spans="1:64" s="3" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="B12" s="37"/>
       <c r="C12" s="30"/>
@@ -2171,7 +2171,7 @@
       </c>
       <c r="G12" s="23"/>
       <c r="H12" s="23">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I12" s="32"/>
@@ -2231,10 +2231,10 @@
       <c r="BK12" s="32"/>
       <c r="BL12" s="32"/>
     </row>
-    <row r="13" spans="1:64" s="3" customFormat="1" ht="21" thickBot="1">
+    <row r="13" spans="1:64" s="3" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
       <c r="B13" s="38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="40"/>
@@ -2242,7 +2242,7 @@
       <c r="F13" s="42"/>
       <c r="G13" s="23"/>
       <c r="H13" s="23" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I13" s="32"/>
@@ -2302,10 +2302,10 @@
       <c r="BK13" s="32"/>
       <c r="BL13" s="32"/>
     </row>
-    <row r="14" spans="1:64" s="3" customFormat="1" ht="21" thickBot="1">
+    <row r="14" spans="1:64" s="3" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="B14" s="43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="44"/>
       <c r="D14" s="45">
@@ -2319,7 +2319,7 @@
       </c>
       <c r="G14" s="23"/>
       <c r="H14" s="23">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I14" s="32"/>
@@ -2379,10 +2379,10 @@
       <c r="BK14" s="32"/>
       <c r="BL14" s="32"/>
     </row>
-    <row r="15" spans="1:64" s="3" customFormat="1" ht="21" thickBot="1">
+    <row r="15" spans="1:64" s="3" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="44"/>
       <c r="D15" s="45">
@@ -2396,7 +2396,7 @@
       </c>
       <c r="G15" s="23"/>
       <c r="H15" s="23">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I15" s="32"/>
@@ -2456,10 +2456,10 @@
       <c r="BK15" s="32"/>
       <c r="BL15" s="32"/>
     </row>
-    <row r="16" spans="1:64" s="3" customFormat="1" ht="21" thickBot="1">
+    <row r="16" spans="1:64" s="3" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="B16" s="48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="44"/>
       <c r="D16" s="45">
@@ -2473,7 +2473,7 @@
       </c>
       <c r="G16" s="23"/>
       <c r="H16" s="23">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I16" s="32"/>
@@ -2533,7 +2533,7 @@
       <c r="BK16" s="32"/>
       <c r="BL16" s="32"/>
     </row>
-    <row r="17" spans="1:64" s="3" customFormat="1" ht="21" thickBot="1">
+    <row r="17" spans="1:64" s="3" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
       <c r="B17" s="48"/>
       <c r="C17" s="44"/>
@@ -2548,7 +2548,7 @@
       </c>
       <c r="G17" s="23"/>
       <c r="H17" s="23">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I17" s="32"/>
@@ -2610,17 +2610,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="J1:AA1"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="J1:AA1"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="BF4:BL4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D9">
     <cfRule type="dataBar" priority="20">
@@ -2847,15 +2847,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004F9D02C8107430489FB053B8051C13E7" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f2e5cfbb6cee37a97a862036e1937735">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8cd4d63e-680a-46bc-8d88-fad229925cc1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="02604a815079e42c3bfd83b4fe82b991" ns2:_="">
     <xsd:import namespace="8cd4d63e-680a-46bc-8d88-fad229925cc1"/>
@@ -2987,14 +2978,46 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{231F19D4-0DA3-465E-A79C-F5342B35E2D7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{231F19D4-0DA3-465E-A79C-F5342B35E2D7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8372004C-6885-41D7-BCF5-6C465EA91F77}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C26A9BA-18AB-429E-86B4-32A430EEDA6F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8cd4d63e-680a-46bc-8d88-fad229925cc1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C26A9BA-18AB-429E-86B4-32A430EEDA6F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8372004C-6885-41D7-BCF5-6C465EA91F77}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>